<commit_message>
change the data set for virus stats
</commit_message>
<xml_diff>
--- a/app/helper/2020_02_21_covid19_country.xlsx
+++ b/app/helper/2020_02_21_covid19_country.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="2020_02_22_covid19_country" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="57">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -165,6 +165,33 @@
   </si>
   <si>
     <t xml:space="preserve">Africa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">total cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total recover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diamon Princess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia (at the Japanese harbour) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
   </si>
 </sst>
 </file>
@@ -179,6 +206,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -262,14 +290,14 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
   </cols>
@@ -752,17 +780,902 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>76940</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>652</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2444</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>23163</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>11477</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>691</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>602</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
update the data resource
</commit_message>
<xml_diff>
--- a/app/helper/2020_02_21_covid19_country.xlsx
+++ b/app/helper/2020_02_21_covid19_country.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2020_02_22_covid19_country" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="2020_02_23_covid19_country" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="64">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -185,13 +186,34 @@
     <t xml:space="preserve">Critical</t>
   </si>
   <si>
-    <t xml:space="preserve">Diamon Princess</t>
+    <t xml:space="preserve">Diamond Princess</t>
   </si>
   <si>
     <t xml:space="preserve">Asia (at the Japanese harbour) </t>
   </si>
   <si>
     <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuwait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afghanistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahrain</t>
   </si>
 </sst>
 </file>
@@ -290,11 +312,11 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
@@ -783,10 +805,14 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.36"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -920,7 +946,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>134</v>
@@ -1024,7 +1050,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>35</v>
@@ -1648,7 +1674,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -1669,6 +1695,1022 @@
         <v>0</v>
       </c>
       <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>77345</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>409</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2593</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>25010</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>11477</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>833</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>691</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the new data
</commit_message>
<xml_diff>
--- a/app/helper/2020_02_21_covid19_country.xlsx
+++ b/app/helper/2020_02_21_covid19_country.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2020_02_22_covid19_country" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="2020_02_23_covid19_country" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2020_02_24_covid19_country" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2020_02_25_covid19_country" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="70">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -214,6 +215,24 @@
   </si>
   <si>
     <t xml:space="preserve">Bahrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diamon Princess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asaia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iraq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coratia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerlan</t>
   </si>
 </sst>
 </file>
@@ -316,7 +335,7 @@
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
@@ -804,11 +823,11 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.36"/>
@@ -1720,7 +1739,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
@@ -2711,6 +2730,1122 @@
         <v>0</v>
       </c>
       <c r="H38" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>77666</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2664</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>27636</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>9126</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>977</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>691</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new data set
</commit_message>
<xml_diff>
--- a/app/helper/2020_02_21_covid19_country.xlsx
+++ b/app/helper/2020_02_21_covid19_country.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2020_02_22_covid19_country" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="2020_02_24_covid19_country" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="2020_02_25_covid19_country" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="2020_02_26_covid19" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="78">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -233,6 +234,30 @@
   </si>
   <si>
     <t xml:space="preserve">Switzerlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new deaths </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia (at Yokohama) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miiddle East </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
   </si>
 </sst>
 </file>
@@ -335,7 +360,7 @@
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
@@ -827,7 +852,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.36"/>
@@ -1739,7 +1764,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
@@ -2751,8 +2776,1124 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>77666</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2664</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>27636</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>9126</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>977</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>691</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H45"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2771,7 +3912,7 @@
         <v>50</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>52</v>
@@ -2788,22 +3929,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>77666</v>
+        <v>78073</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>516</v>
+        <v>415</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2664</v>
+        <v>2715</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>27636</v>
+        <v>30013</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>9126</v>
+        <v>8745</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>5</v>
@@ -2814,19 +3955,19 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>977</v>
+        <v>1261</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>6</v>
@@ -2837,7 +3978,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>691</v>
@@ -2849,16 +3990,16 @@
         <v>4</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,22 +4007,22 @@
         <v>57</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>287</v>
+        <v>374</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>22</v>
@@ -2892,22 +4033,22 @@
         <v>56</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>23</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>7</v>
@@ -2918,19 +4059,19 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0</v>
@@ -2944,7 +4085,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -2956,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>7</v>
@@ -2970,10 +4111,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -2982,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>6</v>
@@ -2996,7 +4137,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3022,10 +4163,10 @@
         <v>58</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
@@ -3034,7 +4175,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
@@ -3048,13 +4189,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
@@ -3071,13 +4212,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
@@ -3086,24 +4227,24 @@
         <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -3112,24 +4253,24 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -3138,24 +4279,24 @@
         <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -3164,24 +4305,24 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -3190,10 +4331,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>22</v>
@@ -3201,65 +4342,65 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -3268,24 +4409,24 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="H20" s="0" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -3294,24 +4435,24 @@
         <v>0</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -3320,24 +4461,24 @@
         <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -3346,50 +4487,50 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
@@ -3398,44 +4539,44 @@
         <v>0</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
@@ -3444,30 +4585,30 @@
         <v>0</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
@@ -3476,18 +4617,18 @@
         <v>0</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>2</v>
@@ -3508,18 +4649,18 @@
         <v>0</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -3534,12 +4675,12 @@
         <v>0</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -3554,24 +4695,24 @@
         <v>0</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -3580,24 +4721,24 @@
         <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>
@@ -3606,18 +4747,18 @@
         <v>0</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -3632,24 +4773,24 @@
         <v>0</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
@@ -3658,18 +4799,18 @@
         <v>0</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -3690,12 +4831,12 @@
         <v>0</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -3716,12 +4857,12 @@
         <v>0</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -3736,18 +4877,18 @@
         <v>0</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -3762,24 +4903,24 @@
         <v>0</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -3788,18 +4929,18 @@
         <v>0</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -3820,32 +4961,110 @@
         <v>0</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="0" t="s">
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the new data set and update the data
</commit_message>
<xml_diff>
--- a/app/helper/2020_02_21_covid19_country.xlsx
+++ b/app/helper/2020_02_21_covid19_country.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="2020_02_25_covid19_country" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="2020_02_26_covid19" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2020_02_27_covid19" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="2020_02_29_covid19" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="97">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -289,6 +290,33 @@
   </si>
   <si>
     <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azerbaijan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Marino</t>
   </si>
 </sst>
 </file>
@@ -388,10 +416,10 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="A1:H52"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="A1:H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
@@ -880,10 +908,10 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A1:H52"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A1:H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.36"/>
@@ -1792,10 +1820,10 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="A1:H52 I15"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="A1:H61 I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
@@ -2808,10 +2836,10 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="1" sqref="A1:H52 M15"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="1" sqref="A1:H61 M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3924,10 +3952,10 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="A1:H52 J24"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="A1:H61 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5117,8 +5145,1384 @@
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>78514</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2747</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>32954</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>8346</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1766</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>705</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>528</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H61"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H52"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5154,22 +6558,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>78514</v>
+        <v>78832</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>450</v>
+        <v>335</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2747</v>
+        <v>2788</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>32954</v>
+        <v>36455</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>8346</v>
+        <v>7952</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>5</v>
@@ -5180,22 +6584,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1766</v>
+        <v>2337</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>505</v>
+        <v>571</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>24</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>7</v>
@@ -5212,16 +6616,16 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>71</v>
@@ -5232,16 +6636,16 @@
         <v>57</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>528</v>
+        <v>655</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>42</v>
@@ -5258,22 +6662,22 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>245</v>
+        <v>388</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>20</v>
@@ -5284,19 +6688,19 @@
         <v>56</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>13</v>
@@ -5313,7 +6717,7 @@
         <v>96</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
@@ -5325,7 +6729,7 @@
         <v>66</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>10</v>
@@ -5336,13 +6740,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0</v>
@@ -5359,13 +6763,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>60</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
@@ -5374,24 +6778,24 @@
         <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>43</v>
-      </c>
       <c r="C11" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
@@ -5400,24 +6804,24 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
@@ -5426,47 +6830,47 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -5478,24 +6882,24 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -5504,24 +6908,24 @@
         <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -5530,24 +6934,24 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -5556,50 +6960,50 @@
         <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
@@ -5608,13 +7012,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,10 +7026,10 @@
         <v>32</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -5634,10 +7038,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>22</v>
@@ -5648,7 +7052,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -5660,7 +7064,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>2</v>
@@ -5671,13 +7075,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -5686,24 +7090,24 @@
         <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -5712,7 +7116,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0</v>
@@ -5723,10 +7127,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0</v>
@@ -5738,47 +7142,47 @@
         <v>0</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="B25" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
@@ -5796,18 +7200,18 @@
         <v>0</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -5822,44 +7226,44 @@
         <v>0</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -5879,13 +7283,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -5905,13 +7309,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -5926,15 +7330,15 @@
         <v>0</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
@@ -5946,47 +7350,47 @@
         <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
@@ -5998,13 +7402,13 @@
         <v>0</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +7416,7 @@
         <v>41</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
@@ -6035,13 +7439,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
@@ -6056,12 +7460,12 @@
         <v>0</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>2</v>
@@ -6076,7 +7480,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>0</v>
@@ -6087,10 +7491,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
@@ -6108,18 +7512,18 @@
         <v>0</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -6134,15 +7538,15 @@
         <v>0</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0</v>
@@ -6154,21 +7558,21 @@
         <v>0</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0</v>
@@ -6180,24 +7584,24 @@
         <v>0</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0</v>
@@ -6206,24 +7610,24 @@
         <v>0</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>0</v>
@@ -6238,18 +7642,18 @@
         <v>0</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>0</v>
@@ -6258,18 +7662,18 @@
         <v>0</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
@@ -6295,7 +7699,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -6310,18 +7714,18 @@
         <v>0</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
@@ -6342,12 +7746,12 @@
         <v>0</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -6368,18 +7772,18 @@
         <v>0</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0</v>
@@ -6394,12 +7798,12 @@
         <v>0</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -6414,24 +7818,24 @@
         <v>0</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
@@ -6440,38 +7844,272 @@
         <v>0</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" s="0" t="s">
+      <c r="B61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>